<commit_message>
Added forms link field, improved efficiency, removed bugs.
</commit_message>
<xml_diff>
--- a/src/form_responses.xlsx
+++ b/src/form_responses.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -45,9 +45,6 @@
     <x:t xml:space="preserve">Last modified time</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">What team are you on?</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">What days are you coming in?</x:t>
   </x:si>
   <x:si>
@@ -60,13 +57,10 @@
     <x:t xml:space="preserve">Shaheer Lone</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">DTS</x:t>
-  </x:si>
-  <x:si>
     <x:t xml:space="preserve">Monday;Wednesday;Thursday;</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">16-W625</x:t>
+    <x:t xml:space="preserve">16-W529</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -163,18 +157,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I3" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:I3"/>
-  <x:tableColumns count="9">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:H2"/>
+  <x:tableColumns count="8">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
     <x:tableColumn id="3" uniqueName="3" name="Completion time" dataDxfId="3"/>
     <x:tableColumn id="4" uniqueName="4" name="Email" dataDxfId="0"/>
     <x:tableColumn id="5" uniqueName="5" name="Name" dataDxfId="0"/>
     <x:tableColumn id="6" uniqueName="6" name="Last modified time" dataDxfId="3"/>
-    <x:tableColumn id="7" uniqueName="7" name="What team are you on?" dataDxfId="0"/>
-    <x:tableColumn id="8" uniqueName="8" name="What days are you coming in?" dataDxfId="0"/>
-    <x:tableColumn id="9" uniqueName="9" name="Choose a desk from the list below:" dataDxfId="0"/>
+    <x:tableColumn id="7" uniqueName="7" name="What days are you coming in?" dataDxfId="0"/>
+    <x:tableColumn id="8" uniqueName="8" name="Choose a desk from the list below:" dataDxfId="0"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -493,7 +486,6 @@
     <x:col min="6" max="6" width="20" hidden="0" bestFit="1" customWidth="1"/>
     <x:col min="7" max="7" width="20" hidden="0" bestFit="1" customWidth="1"/>
     <x:col min="8" max="8" width="20" hidden="0" bestFit="1" customWidth="1"/>
-    <x:col min="9" max="9" width="20" hidden="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" hidden="0">
@@ -521,69 +513,36 @@
       <x:c r="H1" s="10" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="10" t="s">
-        <x:v>8</x:v>
-      </x:c>
     </x:row>
     <x:row r="2" hidden="0">
       <x:c r="A2">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="2">
-        <x:v>45820.6417592593</x:v>
+        <x:v>45828.6792939815</x:v>
       </x:c>
       <x:c r="C2" s="2">
-        <x:v>45820.6420601852</x:v>
+        <x:v>45828.6794675926</x:v>
       </x:c>
       <x:c r="D2" s="10" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="10" t="s">
         <x:v>9</x:v>
-      </x:c>
-      <x:c r="E2" s="10" t="s">
-        <x:v>10</x:v>
       </x:c>
       <x:c r="F2" s="2"/>
       <x:c r="G2" s="10" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H2" s="10" t="s">
         <x:v>11</x:v>
-      </x:c>
-      <x:c r="H2" s="10" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="I2" s="10" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" hidden="0">
-      <x:c r="A3">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="2">
-        <x:v>45820.6422337963</x:v>
-      </x:c>
-      <x:c r="C3" s="2">
-        <x:v>45820.6425347222</x:v>
-      </x:c>
-      <x:c r="D3" s="10" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="E3" s="10" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="F3" s="2"/>
-      <x:c r="G3" s="10" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="H3" s="10" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="I3" s="10" t="s">
-        <x:v>13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R219ef912e0e6440e"/>
+    <x:tablePart r:id="Rc98a8c4558d14c47"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Final touches - app nearly ready for full publishing. Pending presenation to Stephen.
</commit_message>
<xml_diff>
--- a/src/form_responses.xlsx
+++ b/src/form_responses.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -61,6 +61,18 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">16-W529</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">avellingiri@hoopp.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Arulraj Vellingiri</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Monday;Thursday;Friday;</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">16-W625</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -157,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:H2"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H3" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:H3"/>
   <x:tableColumns count="8">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -538,11 +550,35 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
+    <x:row r="3" hidden="0">
+      <x:c r="A3">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="2">
+        <x:v>45831.5861226852</x:v>
+      </x:c>
+      <x:c r="C3" s="2">
+        <x:v>45831.5866319444</x:v>
+      </x:c>
+      <x:c r="D3" s="10" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E3" s="10" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="F3" s="2"/>
+      <x:c r="G3" s="10" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="H3" s="10" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="Rcca2c69f9e434d60"/>
+    <x:tablePart r:id="Rcb063b1b0f154db8"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>